<commit_message>
Finally finished this wornderful experience of usig freest, it was ok
</commit_message>
<xml_diff>
--- a/AnalysisData.xlsx
+++ b/AnalysisData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>Par no gradnularaty</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Seq O(n^2) (s)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>61.464‬</t>
   </si>
 </sst>
 </file>
@@ -86,15 +92,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -377,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G16"/>
+  <dimension ref="A3:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,12 +402,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -433,7 +442,7 @@
       <c r="D5" s="1">
         <v>5.8940000000000001</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.127</v>
       </c>
       <c r="F5" s="1">
@@ -470,6 +479,9 @@
       <c r="C7" s="1">
         <v>100</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E7" s="1">
         <v>0.77200000000000002</v>
       </c>
@@ -487,8 +499,14 @@
       <c r="C8" s="1">
         <v>100</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" s="1">
         <v>7.9379999999999997</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -574,6 +592,352 @@
       </c>
       <c r="E16" s="1">
         <v>45.345999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3">
+        <v>100</v>
+      </c>
+      <c r="C20" s="3">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3">
+        <v>500</v>
+      </c>
+      <c r="C21" s="3">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2.948</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>10</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="3">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4.3630000000000004</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C23" s="3">
+        <v>100</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>37.731000000000002</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>10</v>
+      </c>
+      <c r="B26" s="3">
+        <v>100</v>
+      </c>
+      <c r="C26" s="3">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.56200000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>10</v>
+      </c>
+      <c r="B27" s="3">
+        <v>500</v>
+      </c>
+      <c r="C27" s="3">
+        <v>100</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.83899999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C28" s="3">
+        <v>100</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1.2589999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>10</v>
+      </c>
+      <c r="B29" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C29" s="3">
+        <v>100</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3">
+        <v>8.3040000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>10</v>
+      </c>
+      <c r="B32" s="3">
+        <v>100</v>
+      </c>
+      <c r="C32" s="3">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3">
+        <v>10</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3">
+        <v>500</v>
+      </c>
+      <c r="C33" s="3">
+        <v>100</v>
+      </c>
+      <c r="D33" s="3">
+        <v>5</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.85799999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>10</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C34" s="3">
+        <v>100</v>
+      </c>
+      <c r="D34" s="3">
+        <v>10</v>
+      </c>
+      <c r="E34" s="3">
+        <v>9.0950000000000006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>10</v>
+      </c>
+      <c r="B35" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C35" s="3">
+        <v>100</v>
+      </c>
+      <c r="D35" s="3">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3">
+        <v>79.930999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
+        <v>100</v>
+      </c>
+      <c r="C38" s="3">
+        <v>10</v>
+      </c>
+      <c r="D38" s="3">
+        <v>6</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1.2849999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>10</v>
+      </c>
+      <c r="B39" s="3">
+        <v>500</v>
+      </c>
+      <c r="C39" s="3">
+        <v>100</v>
+      </c>
+      <c r="D39" s="3">
+        <v>5</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C40" s="3">
+        <v>100</v>
+      </c>
+      <c r="D40" s="3">
+        <v>6</v>
+      </c>
+      <c r="E40" s="3">
+        <v>8.9629999999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>10</v>
+      </c>
+      <c r="B41" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C41" s="3">
+        <v>100</v>
+      </c>
+      <c r="D41" s="3">
+        <v>6</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>